<commit_message>
added relocation assistance based on Caliendo et al. (2011)
</commit_message>
<xml_diff>
--- a/estimates/jobSearchInformation.xlsx
+++ b/estimates/jobSearchInformation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19590" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="G8" sheetId="1" r:id="rId1"/>
@@ -898,27 +898,27 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="47.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="47.1328125" customWidth="1"/>
+    <col min="2" max="2" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.59765625" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" customWidth="1"/>
-    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="39.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="33.140625" customWidth="1"/>
-    <col min="13" max="13" width="58.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.73046875" customWidth="1"/>
+    <col min="9" max="9" width="9.265625" customWidth="1"/>
+    <col min="10" max="10" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.73046875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="33.1328125" customWidth="1"/>
+    <col min="13" max="13" width="58.73046875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -959,7 +959,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -976,14 +976,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="K3" s="3"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L5" s="2"/>
     </row>
   </sheetData>

</xml_diff>